<commit_message>
Mostrar datos recibidos en primera celda de excel
</commit_message>
<xml_diff>
--- a/FormatoPM.xlsx
+++ b/FormatoPM.xlsx
@@ -14,7 +14,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="81">
+  <si>
+    <t>Nombre otorgante 1</t>
+  </si>
+  <si>
+    <t>Institucion 1</t>
+  </si>
+  <si>
+    <t>24/05/2023</t>
+  </si>
   <si>
     <t>ENCABEZADO</t>
   </si>
@@ -254,7 +263,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,6 +280,12 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -378,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -409,6 +424,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -705,7 +729,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DB2"/>
+  <dimension ref="A1:DB3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -713,8 +737,8 @@
   <cols>
     <col min="1" max="1" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -811,7 +835,7 @@
   <sheetData>
     <row r="1" spans="1:106" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -821,7 +845,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -850,7 +874,7 @@
       <c r="AH1" s="3"/>
       <c r="AI1" s="3"/>
       <c r="AJ1" s="4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AK1" s="4"/>
       <c r="AL1" s="4"/>
@@ -873,7 +897,7 @@
       <c r="BC1" s="4"/>
       <c r="BD1" s="4"/>
       <c r="BE1" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="BF1" s="5"/>
       <c r="BG1" s="5"/>
@@ -900,14 +924,14 @@
       <c r="CB1" s="5"/>
       <c r="CC1" s="5"/>
       <c r="CD1" s="6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="CE1" s="6"/>
       <c r="CF1" s="6"/>
       <c r="CG1" s="6"/>
       <c r="CH1" s="6"/>
       <c r="CI1" s="7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="CJ1" s="7"/>
       <c r="CK1" s="7"/>
@@ -931,322 +955,346 @@
     </row>
     <row r="2" spans="1:106">
       <c r="A2" s="8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI2" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AS2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AZ2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="BA2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="BB2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="BD2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="BE2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="BF2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="BI2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ2" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="BK2" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="BL2" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="BM2" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="BN2" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="BO2" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BP2" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="BQ2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="BR2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="BS2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="BT2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BU2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="BV2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="BW2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="BX2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="BY2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="BZ2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="CA2" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="CB2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="CC2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="CD2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="CE2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="CF2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="CG2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="CH2" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="CI2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="CJ2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="CK2" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="CL2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="CM2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="CN2" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="CO2" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="CP2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="CQ2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="CR2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="CS2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="CT2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="CU2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="CV2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="CW2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="CX2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="R2" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="U2" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="V2" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="X2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z2" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA2" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE2" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG2" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="AH2" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI2" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="AJ2" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="AL2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM2" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="AO2" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="AP2" s="10" t="s">
+      <c r="CY2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="CZ2" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="AQ2" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="AR2" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS2" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AT2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AU2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="AW2" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="AX2" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AY2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AZ2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="BA2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="BB2" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="BC2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="BD2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE2" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="BF2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="BG2" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="BH2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="BI2" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ2" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="BK2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="BL2" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="BM2" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="BN2" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="BO2" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="BP2" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="BQ2" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="BR2" s="9" t="s">
+      <c r="DA2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="BS2" s="9" t="s">
+      <c r="DB2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="BT2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="BU2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="BV2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="BW2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="BX2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="BY2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="BZ2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="CA2" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="CB2" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="CC2" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="CD2" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="CE2" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="CF2" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="CG2" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="CH2" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="CI2" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="CJ2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="CK2" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="CL2" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="CM2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="CN2" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="CO2" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="CP2" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="CQ2" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="CR2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="CS2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="CT2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="CU2" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="CV2" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="CW2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="CX2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="CY2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="CZ2" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="DA2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="DB2" s="9" t="s">
-        <v>18</v>
+    </row>
+    <row r="3" spans="1:106">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13">
+        <v>3</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14">
+        <v>1</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="14">
+        <v>1</v>
+      </c>
+      <c r="H3" s="14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correccion de validaciones y version 1 acabada
</commit_message>
<xml_diff>
--- a/FormatoPM.xlsx
+++ b/FormatoPM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="140">
   <si>
     <t>ENCABEZADO</t>
   </si>
@@ -250,157 +250,190 @@
     <t>Nombre otorgante 1</t>
   </si>
   <si>
-    <t>Institucion 1</t>
+    <t>Ins</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>24052023</t>
+  </si>
+  <si>
+    <t>042022</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>wwwwwwwwwwwwj</t>
+  </si>
+  <si>
+    <t>saddddddsssssdhsss</t>
+  </si>
+  <si>
+    <t>nombre 1</t>
+  </si>
+  <si>
+    <t>nombre 2</t>
+  </si>
+  <si>
+    <t>eg34567890123456789012345</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t>un</t>
+  </si>
+  <si>
+    <t>asdfghj</t>
+  </si>
+  <si>
+    <t>Leon</t>
+  </si>
+  <si>
+    <t>37006</t>
+  </si>
+  <si>
+    <t>correo@gmail.com</t>
+  </si>
+  <si>
+    <t>nombre21</t>
+  </si>
+  <si>
+    <t>Toluca</t>
+  </si>
+  <si>
+    <t>76215</t>
+  </si>
+  <si>
+    <t>nombre22</t>
+  </si>
+  <si>
+    <t>Tijuana</t>
+  </si>
+  <si>
+    <t>123456789098</t>
+  </si>
+  <si>
+    <t>123456789098765432</t>
+  </si>
+  <si>
+    <t>nombre1</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>ap1</t>
+  </si>
+  <si>
+    <t>3700</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>nombre2</t>
+  </si>
+  <si>
+    <t>ap2</t>
+  </si>
+  <si>
+    <t>456</t>
+  </si>
+  <si>
+    <t>Br</t>
+  </si>
+  <si>
+    <t>nombre3</t>
+  </si>
+  <si>
+    <t>ap3</t>
+  </si>
+  <si>
+    <t>asdfghjklapo2</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>24052023</t>
-  </si>
-  <si>
-    <t>042022</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>MXN</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>asdf</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>wwwwwwwwwwww</t>
-  </si>
-  <si>
-    <t>saddddddsssssdhsss</t>
-  </si>
-  <si>
-    <t>nombre 1</t>
-  </si>
-  <si>
-    <t>nombre 2</t>
-  </si>
-  <si>
-    <t>eg</t>
-  </si>
-  <si>
-    <t>ff</t>
-  </si>
-  <si>
-    <t>mx</t>
-  </si>
-  <si>
-    <t>un</t>
-  </si>
-  <si>
-    <t>Leon</t>
-  </si>
-  <si>
-    <t>37006</t>
-  </si>
-  <si>
-    <t>correo@gmail.com</t>
-  </si>
-  <si>
-    <t>nombre21</t>
-  </si>
-  <si>
-    <t>ahs</t>
-  </si>
-  <si>
-    <t>Toluca</t>
-  </si>
-  <si>
-    <t>76215</t>
-  </si>
-  <si>
-    <t>nombre22</t>
-  </si>
-  <si>
-    <t>Tijuana</t>
-  </si>
-  <si>
-    <t>123456789098</t>
-  </si>
-  <si>
-    <t>123456789098765432</t>
-  </si>
-  <si>
-    <t>nombre1</t>
-  </si>
-  <si>
-    <t>si</t>
-  </si>
-  <si>
-    <t>ap1</t>
-  </si>
-  <si>
-    <t>3700</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>PO</t>
-  </si>
-  <si>
-    <t>nombre2</t>
-  </si>
-  <si>
-    <t>ap2</t>
-  </si>
-  <si>
-    <t>456</t>
-  </si>
-  <si>
-    <t>nombre3</t>
-  </si>
-  <si>
-    <t>ap3</t>
-  </si>
-  <si>
-    <t>asdfghjklapo2</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>20102012</t>
-  </si>
-  <si>
-    <t>MXN</t>
-  </si>
-  <si>
-    <t>08102002</t>
-  </si>
-  <si>
-    <t>05112013</t>
-  </si>
-  <si>
-    <t>23112023</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>22022000</t>
-  </si>
-  <si>
-    <t>23052023</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>asv</t>
+  </si>
+  <si>
+    <t>asdfghjklñzxcvbnml</t>
+  </si>
+  <si>
+    <t>uno</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>gomez</t>
+  </si>
+  <si>
+    <t>asfghjklñzxcvbnmasdqwertyuiopasdfghjklñz</t>
+  </si>
+  <si>
+    <t>37100</t>
+  </si>
+  <si>
+    <t>4776009669</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>rea</t>
+  </si>
+  <si>
+    <t>lira</t>
+  </si>
+  <si>
+    <t>CDMX</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>4778263456</t>
   </si>
 </sst>
 </file>
@@ -897,17 +930,17 @@
     <col min="1" max="1" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -974,18 +1007,21 @@
     <col min="84" max="84" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="85" max="85" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="86" max="86" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="87" max="88" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="89" max="89" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="90" max="91" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="94" max="95" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="40" style="1" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="99" max="99" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="104" max="104" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -1455,8 +1491,8 @@
       <c r="G3" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="H3" s="15" t="s">
-        <v>82</v>
+      <c r="H3" s="15">
+        <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>84</v>
@@ -1483,8 +1519,8 @@
       <c r="Q3" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="R3" s="15" t="s">
-        <v>82</v>
+      <c r="R3" s="15">
+        <v>12345678901</v>
       </c>
       <c r="S3" s="14" t="s">
         <v>82</v>
@@ -1493,7 +1529,7 @@
         <v>82</v>
       </c>
       <c r="U3" s="15" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="V3" s="15" t="s">
         <v>82</v>
@@ -1502,7 +1538,7 @@
         <v>82</v>
       </c>
       <c r="X3" s="15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Y3" s="15" t="s">
         <v>82</v>
@@ -1511,7 +1547,7 @@
         <v>82</v>
       </c>
       <c r="AA3" s="15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AB3" s="14" t="s">
         <v>82</v>
@@ -1535,7 +1571,7 @@
         <v>82</v>
       </c>
       <c r="AI3" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AJ3" s="15" t="s">
         <v>101</v>
@@ -1559,7 +1595,9 @@
       <c r="AQ3" s="15">
         <v>10</v>
       </c>
-      <c r="AR3" s="15"/>
+      <c r="AR3" s="15" t="s">
+        <v>82</v>
+      </c>
       <c r="AS3" s="15" t="s">
         <v>82</v>
       </c>
@@ -1567,7 +1605,7 @@
         <v>82</v>
       </c>
       <c r="AU3" s="15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AV3" s="15" t="s">
         <v>82</v>
@@ -1597,19 +1635,19 @@
         <v>108</v>
       </c>
       <c r="BE3" s="15" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="BF3" s="15">
         <v>1</v>
       </c>
       <c r="BG3" s="15" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="BH3" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="BI3" s="15" t="s">
-        <v>116</v>
+        <v>117</v>
+      </c>
+      <c r="BI3" s="15">
+        <v>20102012</v>
       </c>
       <c r="BJ3" s="16">
         <v>67</v>
@@ -1621,7 +1659,7 @@
         <v>54000</v>
       </c>
       <c r="BM3" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="BN3" s="15">
         <v>7</v>
@@ -1630,15 +1668,15 @@
         <v>7</v>
       </c>
       <c r="BP3" s="16"/>
-      <c r="BQ3" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="BR3" s="14" t="s">
-        <v>119</v>
+      <c r="BQ3" s="15">
+        <v>8102002</v>
+      </c>
+      <c r="BR3" s="14">
+        <v>5112013</v>
       </c>
       <c r="BS3" s="14"/>
-      <c r="BT3" s="14" t="s">
-        <v>120</v>
+      <c r="BT3" s="14">
+        <v>23112023</v>
       </c>
       <c r="BU3" s="14"/>
       <c r="BV3" s="14"/>
@@ -1647,21 +1685,21 @@
       </c>
       <c r="BX3" s="14"/>
       <c r="BY3" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="BZ3" s="15" t="s">
-        <v>122</v>
+        <v>119</v>
+      </c>
+      <c r="BZ3" s="15">
+        <v>22022000</v>
       </c>
       <c r="CA3" s="15"/>
       <c r="CB3" s="16"/>
-      <c r="CC3" s="17" t="s">
+      <c r="CC3" s="17">
+        <v>23052023</v>
+      </c>
+      <c r="CD3" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="CD3" s="15" t="s">
-        <v>127</v>
-      </c>
       <c r="CE3" s="15" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="CF3" s="15">
         <v>34</v>
@@ -1671,6 +1709,66 @@
       </c>
       <c r="CH3" s="15" t="s">
         <v>82</v>
+      </c>
+      <c r="CI3" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="CJ3" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="CK3" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="CL3" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CM3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="CN3" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="CO3" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="CP3" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="CQ3" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CR3" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CS3" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="CT3" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CU3" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CV3" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="CW3" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="CX3" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="CY3" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="CZ3" s="15">
+        <v>2</v>
+      </c>
+      <c r="DA3" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="DB3" s="14" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:106">
@@ -1680,17 +1778,19 @@
       <c r="B4" s="14">
         <v>3</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="15"/>
+      <c r="C4" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>82</v>
+      </c>
       <c r="E4" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>82</v>
-      </c>
+      <c r="F4" s="15"/>
       <c r="G4" s="15"/>
-      <c r="H4" s="15" t="s">
-        <v>82</v>
+      <c r="H4" s="15">
+        <v>87</v>
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="14" t="s">
@@ -1701,10 +1801,10 @@
         <v>82</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="O4" s="14" t="s">
         <v>82</v>
@@ -1787,7 +1887,7 @@
         <v>110</v>
       </c>
       <c r="AQ4" s="15">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="AR4" s="15" t="s">
         <v>82</v>
@@ -1826,14 +1926,14 @@
         <v>82</v>
       </c>
       <c r="BD4" s="14" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="BE4" s="15"/>
       <c r="BF4" s="15">
         <v>2</v>
       </c>
       <c r="BG4" s="15" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="BH4" s="14"/>
       <c r="BI4" s="15"/>
@@ -1841,7 +1941,7 @@
       <c r="BK4" s="15"/>
       <c r="BL4" s="15"/>
       <c r="BM4" s="15" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="BN4" s="15">
         <v>10</v>
@@ -1862,14 +1962,12 @@
       <c r="BZ4" s="15"/>
       <c r="CA4" s="15"/>
       <c r="CB4" s="16"/>
-      <c r="CC4" s="17" t="s">
-        <v>123</v>
-      </c>
+      <c r="CC4" s="17"/>
       <c r="CD4" s="15" t="s">
         <v>82</v>
       </c>
       <c r="CE4" s="15" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
       <c r="CF4" s="15">
         <v>45</v>
@@ -1878,15 +1976,73 @@
         <v>2</v>
       </c>
       <c r="CH4" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CI4" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="CJ4" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="CK4" s="15"/>
+      <c r="CL4" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CM4" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CN4" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="CO4" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="CP4" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CQ4" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CR4" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CS4" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="CT4" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CU4" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CV4" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="CW4" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="CX4" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="CY4" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="CZ4" s="15">
+        <v>3</v>
+      </c>
+      <c r="DA4" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="DB4" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:106">
       <c r="A5" s="13">
-        <v>3</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>82</v>
+        <v>1234</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1234</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>82</v>
@@ -1897,9 +2053,7 @@
       <c r="E5" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>82</v>
-      </c>
+      <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15" t="s">
         <v>82</v>
@@ -1987,13 +2141,13 @@
       </c>
       <c r="AL5" s="15"/>
       <c r="AM5" s="15" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AN5" s="15" t="s">
         <v>82</v>
       </c>
       <c r="AO5" s="15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AP5" s="15" t="s">
         <v>82</v>
@@ -2051,7 +2205,7 @@
       <c r="BK5" s="15"/>
       <c r="BL5" s="15"/>
       <c r="BM5" s="15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="BN5" s="15"/>
       <c r="BO5" s="16"/>
@@ -2068,14 +2222,12 @@
       <c r="BZ5" s="15"/>
       <c r="CA5" s="15"/>
       <c r="CB5" s="16"/>
-      <c r="CC5" s="17" t="s">
-        <v>123</v>
-      </c>
+      <c r="CC5" s="17"/>
       <c r="CD5" s="15" t="s">
         <v>82</v>
       </c>
       <c r="CE5" s="15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="CF5" s="15">
         <v>68</v>
@@ -2084,6 +2236,64 @@
         <v>82</v>
       </c>
       <c r="CH5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CI5" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="CJ5" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="CK5" s="15"/>
+      <c r="CL5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CM5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CN5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CO5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CP5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CQ5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CR5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CS5" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="CT5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CU5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CV5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="CW5" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="CX5" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="CY5" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="CZ5" s="15">
+        <v>1</v>
+      </c>
+      <c r="DA5" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="DB5" s="14" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Formato PM resumido de codigo
</commit_message>
<xml_diff>
--- a/FormatoPM.xlsx
+++ b/FormatoPM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="176">
   <si>
     <t>ENCABEZADO</t>
   </si>
@@ -292,15 +292,60 @@
     <t>asdfghj</t>
   </si>
   <si>
+    <t>Leon 1</t>
+  </si>
+  <si>
     <t>Leon</t>
   </si>
   <si>
+    <t>Monterrey</t>
+  </si>
+  <si>
+    <t>Nuev</t>
+  </si>
+  <si>
+    <t>37006</t>
+  </si>
+  <si>
+    <t>4231023847</t>
+  </si>
+  <si>
+    <t>54132</t>
+  </si>
+  <si>
+    <t>9864531</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>Fi</t>
+  </si>
+  <si>
+    <t>12378921</t>
+  </si>
+  <si>
+    <t>correo@gmail.com</t>
+  </si>
+  <si>
     <t>nombre21</t>
   </si>
   <si>
     <t>Toluca</t>
   </si>
   <si>
+    <t>76215</t>
+  </si>
+  <si>
+    <t>21307982</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Es</t>
+  </si>
+  <si>
     <t>nombre22</t>
   </si>
   <si>
@@ -322,15 +367,36 @@
     <t>ap1</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>direccion 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> direccion 2</t>
+  </si>
+  <si>
+    <t>Valle de León</t>
+  </si>
+  <si>
+    <t>Ciudad Victoria</t>
+  </si>
+  <si>
+    <t>GRO</t>
   </si>
   <si>
     <t>3700</t>
   </si>
   <si>
+    <t>46548645</t>
+  </si>
+  <si>
     <t>123</t>
   </si>
   <si>
+    <t>789452</t>
+  </si>
+  <si>
+    <t>Edo extranjero 1</t>
+  </si>
+  <si>
     <t>PO</t>
   </si>
   <si>
@@ -340,12 +406,12 @@
     <t>ap2</t>
   </si>
   <si>
-    <t>76215</t>
-  </si>
-  <si>
     <t>456</t>
   </si>
   <si>
+    <t>Edo extranjero 2</t>
+  </si>
+  <si>
     <t>Br</t>
   </si>
   <si>
@@ -358,30 +424,48 @@
     <t>asdfghjklapo2</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>5</t>
+    <t>20102012</t>
   </si>
   <si>
     <t>MXN</t>
   </si>
   <si>
+    <t>08102002</t>
+  </si>
+  <si>
+    <t>05112013</t>
+  </si>
+  <si>
+    <t>23112023</t>
+  </si>
+  <si>
+    <t>Hola</t>
+  </si>
+  <si>
     <t>F</t>
   </si>
   <si>
+    <t>22022000</t>
+  </si>
+  <si>
+    <t>23052023</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>Ejem</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -403,7 +487,20 @@
     <t>gomez</t>
   </si>
   <si>
-    <t>asfghjklñzxcvbnmasdqwertyuiopasdfghjklñz</t>
+    <t>asfghjklñzxcvbnmasdq
+wertyuiopasdfghjklñz</t>
+  </si>
+  <si>
+    <t>dire2</t>
+  </si>
+  <si>
+    <t>La india</t>
+  </si>
+  <si>
+    <t>city1</t>
+  </si>
+  <si>
+    <t>CHIH</t>
   </si>
   <si>
     <t>37100</t>
@@ -412,6 +509,13 @@
     <t>4776009669</t>
   </si>
   <si>
+    <t>123908</t>
+  </si>
+  <si>
+    <t>texto tan grande que
+supera los 40 carac</t>
+  </si>
+  <si>
     <t>asd</t>
   </si>
   <si>
@@ -424,10 +528,22 @@
     <t>CDMX</t>
   </si>
   <si>
+    <t>city2</t>
+  </si>
+  <si>
     <t>123456</t>
   </si>
   <si>
     <t>4778263456</t>
+  </si>
+  <si>
+    <t>Al</t>
+  </si>
+  <si>
+    <t>nombre4</t>
+  </si>
+  <si>
+    <t>nombre5</t>
   </si>
 </sst>
 </file>
@@ -915,7 +1031,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DB6"/>
+  <dimension ref="A1:DB7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -942,17 +1058,17 @@
     <col min="21" max="22" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -960,17 +1076,18 @@
     <col min="41" max="41" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -1007,8 +1124,7 @@
     <col min="90" max="90" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="91" max="91" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="40" style="1" bestFit="1" customWidth="1"/>
+    <col min="93" max="94" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="11" style="1" bestFit="1" customWidth="1"/>
@@ -1017,9 +1133,9 @@
     <col min="100" max="100" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="101" max="101" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="104" max="104" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="106" max="106" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1516,92 +1632,130 @@
       <c r="R3" s="15">
         <v>12345678901</v>
       </c>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
+      <c r="S3" s="14">
+        <v>1234</v>
+      </c>
+      <c r="T3" s="14">
+        <v>67843</v>
+      </c>
       <c r="U3" s="15" t="s">
         <v>91</v>
       </c>
       <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
+      <c r="W3" s="15" t="s">
+        <v>92</v>
+      </c>
       <c r="X3" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y3" s="15"/>
+        <v>93</v>
+      </c>
+      <c r="Y3" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z3" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB3" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC3" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD3" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE3" s="15">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG3" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH3" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI3" s="17" t="s">
+        <v>103</v>
+      </c>
       <c r="AJ3" s="15" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="AK3" s="14" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="AL3" s="15"/>
       <c r="AM3" s="15" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="AN3" s="15" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="AO3" s="15" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="AP3" s="15" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="AQ3" s="15">
         <v>10</v>
       </c>
       <c r="AR3" s="15" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="AS3" s="15" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="AT3" s="15" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="AU3" s="15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AV3" s="15" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="AW3" s="15" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="AX3" s="15" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="AY3" s="14" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="AZ3" s="14" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="BA3" s="14" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="BB3" s="15">
         <v>1</v>
       </c>
       <c r="BC3" s="14" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="BD3" s="14" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="BE3" s="15" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="BF3" s="15">
         <v>1</v>
       </c>
-      <c r="BG3" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="BH3" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="BI3" s="15">
-        <v>20102012</v>
+      <c r="BG3" s="15">
+        <v>1</v>
+      </c>
+      <c r="BH3" s="14">
+        <v>5</v>
+      </c>
+      <c r="BI3" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="BJ3" s="16">
         <v>67</v>
@@ -1613,7 +1767,7 @@
         <v>54000</v>
       </c>
       <c r="BM3" s="15" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="BN3" s="15">
         <v>7</v>
@@ -1621,39 +1775,51 @@
       <c r="BO3" s="16">
         <v>7</v>
       </c>
-      <c r="BP3" s="16"/>
-      <c r="BQ3" s="15">
-        <v>8102002</v>
-      </c>
-      <c r="BR3" s="14">
-        <v>5112013</v>
+      <c r="BP3" s="16">
+        <v>875</v>
+      </c>
+      <c r="BQ3" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="BR3" s="14" t="s">
+        <v>139</v>
       </c>
       <c r="BS3" s="14"/>
-      <c r="BT3" s="14">
-        <v>23112023</v>
-      </c>
-      <c r="BU3" s="14"/>
-      <c r="BV3" s="14"/>
+      <c r="BT3" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="BU3" s="14">
+        <v>123</v>
+      </c>
+      <c r="BV3" s="14">
+        <v>76547</v>
+      </c>
       <c r="BW3" s="14">
         <v>1234</v>
       </c>
-      <c r="BX3" s="14"/>
+      <c r="BX3" s="14" t="s">
+        <v>141</v>
+      </c>
       <c r="BY3" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="BZ3" s="15">
-        <v>22022000</v>
-      </c>
-      <c r="CA3" s="15"/>
-      <c r="CB3" s="16"/>
-      <c r="CC3" s="17">
-        <v>23052023</v>
+        <v>142</v>
+      </c>
+      <c r="BZ3" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="CA3" s="15">
+        <v>200000</v>
+      </c>
+      <c r="CB3" s="16">
+        <v>123098</v>
+      </c>
+      <c r="CC3" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="CD3" s="15" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="CE3" s="15" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="CF3" s="15">
         <v>34</v>
@@ -1661,68 +1827,68 @@
       <c r="CG3" s="15">
         <v>1</v>
       </c>
-      <c r="CH3" s="15" t="s">
-        <v>102</v>
+      <c r="CH3" s="15">
+        <v>123456</v>
       </c>
       <c r="CI3" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="CJ3" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="CK3" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="CL3" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="CM3" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="CN3" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="CO3" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="CP3" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="CQ3" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="CR3" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="CS3" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="CT3" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="CU3" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="CV3" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="CW3" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="CX3" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="CJ3" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="CK3" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="CL3" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CM3" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="CN3" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="CO3" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="CP3" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="CQ3" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CR3" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CS3" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="CT3" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CU3" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CV3" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="CW3" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="CX3" s="14" t="s">
-        <v>102</v>
-      </c>
       <c r="CY3" s="14" t="s">
-        <v>102</v>
+        <v>164</v>
       </c>
       <c r="CZ3" s="15">
         <v>2</v>
       </c>
       <c r="DA3" s="14" t="s">
-        <v>102</v>
+        <v>165</v>
       </c>
       <c r="DB3" s="14" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:106">
@@ -1747,7 +1913,7 @@
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
       <c r="M4" s="15" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="N4" s="14"/>
       <c r="O4" s="14"/>
@@ -1760,74 +1926,76 @@
       <c r="V4" s="15"/>
       <c r="W4" s="15"/>
       <c r="X4" s="15" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB4" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="15">
+        <v>2</v>
+      </c>
+      <c r="AF4" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="AG4" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH4" s="17"/>
+      <c r="AI4" s="17"/>
       <c r="AJ4" s="15"/>
-      <c r="AK4" s="14" t="s">
-        <v>102</v>
-      </c>
+      <c r="AK4" s="14"/>
       <c r="AL4" s="15"/>
       <c r="AM4" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="AN4" s="15" t="s">
-        <v>102</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="AN4" s="15"/>
       <c r="AO4" s="15" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="AP4" s="15" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="AQ4" s="15">
         <v>15</v>
       </c>
-      <c r="AR4" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="AS4" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="AT4" s="15" t="s">
-        <v>102</v>
-      </c>
+      <c r="AR4" s="15"/>
+      <c r="AS4" s="15"/>
+      <c r="AT4" s="15"/>
       <c r="AU4" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AV4" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="AW4" s="15" t="s">
-        <v>102</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="AV4" s="15"/>
+      <c r="AW4" s="15"/>
       <c r="AX4" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="AY4" s="14" t="s">
-        <v>102</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="AY4" s="14"/>
       <c r="AZ4" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="BA4" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="BB4" s="15" t="s">
-        <v>102</v>
+        <v>130</v>
+      </c>
+      <c r="BA4" s="14"/>
+      <c r="BB4" s="15">
+        <v>4</v>
       </c>
       <c r="BC4" s="14" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="BD4" s="14" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="BE4" s="15"/>
       <c r="BF4" s="15">
         <v>2</v>
       </c>
-      <c r="BG4" s="15" t="s">
-        <v>118</v>
+      <c r="BG4" s="15">
+        <v>2</v>
       </c>
       <c r="BH4" s="14"/>
       <c r="BI4" s="15"/>
@@ -1835,7 +2003,7 @@
       <c r="BK4" s="15"/>
       <c r="BL4" s="15"/>
       <c r="BM4" s="15" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="BN4" s="15">
         <v>10</v>
@@ -1846,22 +2014,26 @@
       <c r="BR4" s="14"/>
       <c r="BS4" s="14"/>
       <c r="BT4" s="14"/>
-      <c r="BU4" s="14"/>
-      <c r="BV4" s="14"/>
+      <c r="BU4" s="14">
+        <v>4645</v>
+      </c>
+      <c r="BV4" s="14">
+        <v>98651</v>
+      </c>
       <c r="BW4" s="14">
         <v>4567</v>
       </c>
-      <c r="BX4" s="14"/>
+      <c r="BX4" s="14" t="s">
+        <v>146</v>
+      </c>
       <c r="BY4" s="14"/>
       <c r="BZ4" s="15"/>
       <c r="CA4" s="15"/>
       <c r="CB4" s="16"/>
       <c r="CC4" s="17"/>
-      <c r="CD4" s="15" t="s">
-        <v>102</v>
-      </c>
+      <c r="CD4" s="15"/>
       <c r="CE4" s="15" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="CF4" s="15">
         <v>45</v>
@@ -1869,66 +2041,46 @@
       <c r="CG4" s="15">
         <v>2</v>
       </c>
-      <c r="CH4" s="15" t="s">
-        <v>102</v>
-      </c>
+      <c r="CH4" s="15"/>
       <c r="CI4" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="CJ4" s="14" t="s">
-        <v>102</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="CJ4" s="14"/>
       <c r="CK4" s="15"/>
       <c r="CL4" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CM4" s="15" t="s">
-        <v>102</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="CM4" s="15"/>
       <c r="CN4" s="15" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="CO4" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="CP4" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CQ4" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CR4" s="15" t="s">
-        <v>102</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="CP4" s="15"/>
+      <c r="CQ4" s="15"/>
+      <c r="CR4" s="15"/>
       <c r="CS4" s="15" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="CT4" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CU4" s="15" t="s">
-        <v>102</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="CU4" s="15"/>
       <c r="CV4" s="15" t="s">
-        <v>136</v>
+        <v>171</v>
       </c>
       <c r="CW4" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="CX4" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="CY4" s="14" t="s">
-        <v>102</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="CX4" s="14"/>
+      <c r="CY4" s="14"/>
       <c r="CZ4" s="15">
         <v>3</v>
       </c>
-      <c r="DA4" s="14" t="s">
-        <v>102</v>
-      </c>
+      <c r="DA4" s="14"/>
       <c r="DB4" s="14" t="s">
-        <v>102</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:106">
@@ -1949,7 +2101,7 @@
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
       <c r="M5" s="15" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="N5" s="14"/>
       <c r="O5" s="14"/>
@@ -1962,68 +2114,46 @@
       <c r="V5" s="15"/>
       <c r="W5" s="15"/>
       <c r="X5" s="15" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="15"/>
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="15"/>
+      <c r="AH5" s="17"/>
+      <c r="AI5" s="17"/>
       <c r="AJ5" s="15"/>
-      <c r="AK5" s="14" t="s">
-        <v>102</v>
-      </c>
+      <c r="AK5" s="14"/>
       <c r="AL5" s="15"/>
       <c r="AM5" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="AN5" s="15"/>
+      <c r="AO5" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="AP5" s="15"/>
+      <c r="AQ5" s="15"/>
+      <c r="AR5" s="15"/>
+      <c r="AS5" s="15"/>
+      <c r="AT5" s="15"/>
+      <c r="AU5" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="AN5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO5" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="AP5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="AQ5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="AR5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="AS5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="AT5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="AU5" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="AV5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="AW5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="AX5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="AY5" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="AZ5" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="BA5" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="BB5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="BC5" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="BD5" s="14" t="s">
-        <v>102</v>
-      </c>
+      <c r="AV5" s="15"/>
+      <c r="AW5" s="15"/>
+      <c r="AX5" s="15"/>
+      <c r="AY5" s="14"/>
+      <c r="AZ5" s="14"/>
+      <c r="BA5" s="14"/>
+      <c r="BB5" s="15"/>
+      <c r="BC5" s="14"/>
+      <c r="BD5" s="14"/>
       <c r="BE5" s="15"/>
       <c r="BF5" s="15">
         <v>3</v>
@@ -2035,7 +2165,7 @@
       <c r="BK5" s="15"/>
       <c r="BL5" s="15"/>
       <c r="BM5" s="15" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="BN5" s="15"/>
       <c r="BO5" s="16"/>
@@ -2053,79 +2183,43 @@
       <c r="CA5" s="15"/>
       <c r="CB5" s="16"/>
       <c r="CC5" s="17"/>
-      <c r="CD5" s="15" t="s">
-        <v>102</v>
-      </c>
+      <c r="CD5" s="15"/>
       <c r="CE5" s="15" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="CF5" s="15">
         <v>68</v>
       </c>
-      <c r="CG5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CH5" s="15" t="s">
-        <v>102</v>
-      </c>
+      <c r="CG5" s="15"/>
+      <c r="CH5" s="15"/>
       <c r="CI5" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="CJ5" s="14" t="s">
-        <v>102</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="CJ5" s="14"/>
       <c r="CK5" s="15"/>
       <c r="CL5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CM5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CN5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CO5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CP5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CQ5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CR5" s="15" t="s">
-        <v>102</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="CM5" s="15"/>
+      <c r="CN5" s="15"/>
+      <c r="CO5" s="15"/>
+      <c r="CP5" s="15"/>
+      <c r="CQ5" s="15"/>
+      <c r="CR5" s="15"/>
       <c r="CS5" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="CT5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CU5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CV5" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="CW5" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="CX5" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="CY5" s="14" t="s">
-        <v>102</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="CT5" s="15"/>
+      <c r="CU5" s="15"/>
+      <c r="CV5" s="15"/>
+      <c r="CW5" s="14"/>
+      <c r="CX5" s="14"/>
+      <c r="CY5" s="14"/>
       <c r="CZ5" s="15">
         <v>1</v>
       </c>
-      <c r="DA5" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="DB5" s="14" t="s">
-        <v>102</v>
-      </c>
+      <c r="DA5" s="14"/>
+      <c r="DB5" s="14"/>
     </row>
     <row r="6" spans="1:106">
       <c r="A6" s="13">
@@ -2155,6 +2249,199 @@
       <c r="W6" s="15"/>
       <c r="X6" s="15"/>
       <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="15"/>
+      <c r="AF6" s="14"/>
+      <c r="AG6" s="15"/>
+      <c r="AH6" s="17"/>
+      <c r="AI6" s="17"/>
+      <c r="AJ6" s="15"/>
+      <c r="AK6" s="14"/>
+      <c r="AL6" s="15"/>
+      <c r="AM6" s="15"/>
+      <c r="AN6" s="15"/>
+      <c r="AO6" s="15"/>
+      <c r="AP6" s="15"/>
+      <c r="AQ6" s="15"/>
+      <c r="AR6" s="15"/>
+      <c r="AS6" s="15"/>
+      <c r="AT6" s="15"/>
+      <c r="AU6" s="15"/>
+      <c r="AV6" s="15"/>
+      <c r="AW6" s="15"/>
+      <c r="AX6" s="15"/>
+      <c r="AY6" s="14"/>
+      <c r="AZ6" s="14"/>
+      <c r="BA6" s="14"/>
+      <c r="BB6" s="15"/>
+      <c r="BC6" s="14"/>
+      <c r="BD6" s="14"/>
+      <c r="BE6" s="15"/>
+      <c r="BF6" s="15"/>
+      <c r="BG6" s="15"/>
+      <c r="BH6" s="14"/>
+      <c r="BI6" s="15"/>
+      <c r="BJ6" s="16"/>
+      <c r="BK6" s="15"/>
+      <c r="BL6" s="15"/>
+      <c r="BM6" s="15"/>
+      <c r="BN6" s="15"/>
+      <c r="BO6" s="16"/>
+      <c r="BP6" s="16"/>
+      <c r="BQ6" s="15"/>
+      <c r="BR6" s="14"/>
+      <c r="BS6" s="14"/>
+      <c r="BT6" s="14"/>
+      <c r="BU6" s="14"/>
+      <c r="BV6" s="14"/>
+      <c r="BW6" s="14"/>
+      <c r="BX6" s="14"/>
+      <c r="BY6" s="14"/>
+      <c r="BZ6" s="15"/>
+      <c r="CA6" s="15"/>
+      <c r="CB6" s="16"/>
+      <c r="CC6" s="17"/>
+      <c r="CD6" s="15"/>
+      <c r="CE6" s="15"/>
+      <c r="CF6" s="15"/>
+      <c r="CG6" s="15"/>
+      <c r="CH6" s="15"/>
+      <c r="CI6" s="15"/>
+      <c r="CJ6" s="14"/>
+      <c r="CK6" s="15"/>
+      <c r="CL6" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="CM6" s="15"/>
+      <c r="CN6" s="15"/>
+      <c r="CO6" s="15"/>
+      <c r="CP6" s="15"/>
+      <c r="CQ6" s="15"/>
+      <c r="CR6" s="15"/>
+      <c r="CS6" s="15"/>
+      <c r="CT6" s="15"/>
+      <c r="CU6" s="15"/>
+      <c r="CV6" s="15"/>
+      <c r="CW6" s="14"/>
+      <c r="CX6" s="14"/>
+      <c r="CY6" s="14"/>
+      <c r="CZ6" s="15"/>
+      <c r="DA6" s="14"/>
+      <c r="DB6" s="14"/>
+    </row>
+    <row r="7" spans="1:106">
+      <c r="A7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="14"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="14"/>
+      <c r="AE7" s="15"/>
+      <c r="AF7" s="14"/>
+      <c r="AG7" s="15"/>
+      <c r="AH7" s="17"/>
+      <c r="AI7" s="17"/>
+      <c r="AJ7" s="15"/>
+      <c r="AK7" s="14"/>
+      <c r="AL7" s="15"/>
+      <c r="AM7" s="15"/>
+      <c r="AN7" s="15"/>
+      <c r="AO7" s="15"/>
+      <c r="AP7" s="15"/>
+      <c r="AQ7" s="15"/>
+      <c r="AR7" s="15"/>
+      <c r="AS7" s="15"/>
+      <c r="AT7" s="15"/>
+      <c r="AU7" s="15"/>
+      <c r="AV7" s="15"/>
+      <c r="AW7" s="15"/>
+      <c r="AX7" s="15"/>
+      <c r="AY7" s="14"/>
+      <c r="AZ7" s="14"/>
+      <c r="BA7" s="14"/>
+      <c r="BB7" s="15"/>
+      <c r="BC7" s="14"/>
+      <c r="BD7" s="14"/>
+      <c r="BE7" s="15"/>
+      <c r="BF7" s="15"/>
+      <c r="BG7" s="15"/>
+      <c r="BH7" s="14"/>
+      <c r="BI7" s="15"/>
+      <c r="BJ7" s="16"/>
+      <c r="BK7" s="15"/>
+      <c r="BL7" s="15"/>
+      <c r="BM7" s="15"/>
+      <c r="BN7" s="15"/>
+      <c r="BO7" s="16"/>
+      <c r="BP7" s="16"/>
+      <c r="BQ7" s="15"/>
+      <c r="BR7" s="14"/>
+      <c r="BS7" s="14"/>
+      <c r="BT7" s="14"/>
+      <c r="BU7" s="14"/>
+      <c r="BV7" s="14"/>
+      <c r="BW7" s="14"/>
+      <c r="BX7" s="14"/>
+      <c r="BY7" s="14"/>
+      <c r="BZ7" s="15"/>
+      <c r="CA7" s="15"/>
+      <c r="CB7" s="16"/>
+      <c r="CC7" s="17"/>
+      <c r="CD7" s="15"/>
+      <c r="CE7" s="15"/>
+      <c r="CF7" s="15"/>
+      <c r="CG7" s="15"/>
+      <c r="CH7" s="15"/>
+      <c r="CI7" s="15"/>
+      <c r="CJ7" s="14"/>
+      <c r="CK7" s="15"/>
+      <c r="CL7" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="CM7" s="15"/>
+      <c r="CN7" s="15"/>
+      <c r="CO7" s="15"/>
+      <c r="CP7" s="15"/>
+      <c r="CQ7" s="15"/>
+      <c r="CR7" s="15"/>
+      <c r="CS7" s="15"/>
+      <c r="CT7" s="15"/>
+      <c r="CU7" s="15"/>
+      <c r="CV7" s="15"/>
+      <c r="CW7" s="14"/>
+      <c r="CX7" s="14"/>
+      <c r="CY7" s="14"/>
+      <c r="CZ7" s="15"/>
+      <c r="DA7" s="14"/>
+      <c r="DB7" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>